<commit_message>
update seems_to_be_all_node but not very good
</commit_message>
<xml_diff>
--- a/benchmark/parallel_benchmark.xlsx
+++ b/benchmark/parallel_benchmark.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\egaroucid\Egaroucid\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D2C165-2263-45AE-BB68-E87801D2F3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CCA293-4546-4A8F-B3C8-DE50B6973DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50784" yWindow="5340" windowWidth="34560" windowHeight="18600" xr2:uid="{75C047C0-BFEA-499F-BA8B-EB1F29873334}"/>
+    <workbookView xWindow="50496" yWindow="2220" windowWidth="34560" windowHeight="18600" activeTab="3" xr2:uid="{75C047C0-BFEA-499F-BA8B-EB1F29873334}"/>
   </bookViews>
   <sheets>
     <sheet name="20230602" sheetId="16" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="39">
   <si>
     <t>スレッド数 p(個)</t>
     <rPh sb="4" eb="5">
@@ -41258,8 +41258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A0E446-DB5D-473F-AE24-C5B4318489FE}">
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -47948,8 +47948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56F58585-9DDD-4F71-B3A8-D5BE3FB1AB35}">
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:L3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -48117,6 +48117,13 @@
       <c r="I4">
         <f t="shared" si="3"/>
         <v>0.9130324607173258</v>
+      </c>
+      <c r="K4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4">
+        <f>MAX(E:E)</f>
+        <v>6.2726226993865035</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.45">

</xml_diff>